<commit_message>
foi feito a alteraçao no formulario "manter editora"
foi feito a alteraçao no formulario "manter editora"
</commit_message>
<xml_diff>
--- a/tarefas/ativas/ers/ers-biblioteca-godofredo-20200514-lucas.xlsx
+++ b/tarefas/ativas/ers/ers-biblioteca-godofredo-20200514-lucas.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -394,6 +394,17 @@
 1 botao para salvar as alteraçoes 
 1 butao para fazer a inclusao de um novo autor 
 1 butao para fazer a exclusao de um novo autor 
+1 botao para cancelar a operaçao e voltar ao menu principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+O titulo principal do formulario sera "editora"
+o formulario deve permitoir alterar o cadastro da editora , salvar alteraçoes e cancelar a operaçao e voltar para o menu pricipal , a inclusao e a exclusao de editoras 
+o formulsrio deve conter
+1 campo String  noome da editora 
+1 botao para fazer salvar as alteraçoes 
+1 butao para fazer a inclusao de um nova editora 
+1 butao para fazer a exclusao de um nova editora
 1 botao para cancelar a operaçao e voltar ao menu principal</t>
   </si>
 </sst>
@@ -2888,10 +2899,10 @@
   <dimension ref="A6:J33"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,14 +3045,16 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="22" t="s">
         <v>86</v>
       </c>
       <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="E12" s="35" t="s">
+        <v>110</v>
+      </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25" t="s">

</xml_diff>